<commit_message>
fixed code review issues (#SHEET-222)
Change-Id: Ifeda5b49e841f17d43a85a10c653306cdefe9885
</commit_message>
<xml_diff>
--- a/src/main/resources/testsheets/Embedded Charts.xlsx
+++ b/src/main/resources/testsheets/Embedded Charts.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Edit this spreadsheet to alter embedded chart title and data</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -32,6 +29,9 @@
   </si>
   <si>
     <t>Brand 3</t>
+  </si>
+  <si>
+    <t>Edit this spreadsheet to alter embedded chart data</t>
   </si>
 </sst>
 </file>
@@ -47,12 +47,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -67,8 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -292,11 +306,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="60989952"/>
-        <c:axId val="87660160"/>
+        <c:axId val="60280832"/>
+        <c:axId val="98473600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60989952"/>
+        <c:axId val="60280832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,7 +319,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87660160"/>
+        <c:crossAx val="98473600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -313,7 +327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87660160"/>
+        <c:axId val="98473600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +338,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60989952"/>
+        <c:crossAx val="60280832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -697,46 +711,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>25</v>

</xml_diff>